<commit_message>
Correction Bug ecriture fichier XLSX
correction d un bug d affichage dans le fichier d exportation des resultats (formatage de cellule incorrecte)
</commit_message>
<xml_diff>
--- a/ConfigTower/Template.xlsx
+++ b/ConfigTower/Template.xlsx
@@ -83,9 +83,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY\ HH:MM"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YYYY\ HH:MM"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -274,7 +275,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -295,6 +296,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -303,7 +308,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -443,7 +452,7 @@
   <dimension ref="B4:E36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -481,29 +490,29 @@
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
@@ -514,98 +523,98 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="11" t="n">
+      <c r="B16" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="14" t="n">
+      <c r="B17" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11" t="n">
+      <c r="B18" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="14" t="n">
+      <c r="B19" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="11" t="n">
+      <c r="B20" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="14" t="n">
+      <c r="B21" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="11" t="n">
+      <c r="B22" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="14" t="n">
+      <c r="B23" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="11" t="n">
+      <c r="B24" s="13" t="n">
         <v>9</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="17" t="n">
+      <c r="B25" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
     </row>
     <row r="30" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2" t="s">
@@ -619,42 +628,42 @@
         <v>13</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="20"/>
+      <c r="D31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="20"/>
+      <c r="D32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="20"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="20"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="19"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="21"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="19"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>